<commit_message>
New sprites and added all Pokemon for main story!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Microsoft\Excel\Pokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656EB625-4973-4024-A49F-4EB323C14958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF132A83-5B4C-4510-A9B7-F535FF001517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="254">
   <si>
     <t>Current</t>
   </si>
@@ -669,6 +670,135 @@
   </si>
   <si>
     <t>POSTGAME</t>
+  </si>
+  <si>
+    <t>Afterwords, find some reason to go back to the lab to talk to your dad and get your dex upgraded for E pokemon</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>1st gate</t>
+  </si>
+  <si>
+    <t>Scott 1</t>
+  </si>
+  <si>
+    <t>Rick 1</t>
+  </si>
+  <si>
+    <t>Sicab Office</t>
+  </si>
+  <si>
+    <t>Scott 2</t>
+  </si>
+  <si>
+    <t>Fred 2</t>
+  </si>
+  <si>
+    <t>Key A</t>
+  </si>
+  <si>
+    <t>Key B</t>
+  </si>
+  <si>
+    <t>Room A</t>
+  </si>
+  <si>
+    <t>Room B</t>
+  </si>
+  <si>
+    <t>Gift Starter</t>
+  </si>
+  <si>
+    <t>Gift Dog</t>
+  </si>
+  <si>
+    <t>Gift Magic</t>
+  </si>
+  <si>
+    <t>Gift Fossil</t>
+  </si>
+  <si>
+    <t>Gift "Starter"</t>
+  </si>
+  <si>
+    <t>Scott 3</t>
+  </si>
+  <si>
+    <t>Grandpa</t>
+  </si>
+  <si>
+    <t>Gym 5</t>
+  </si>
+  <si>
+    <t>Gift E/S</t>
+  </si>
+  <si>
+    <t>Rick 2</t>
+  </si>
+  <si>
+    <t>Maxwell 1</t>
+  </si>
+  <si>
+    <t>Scott 4</t>
+  </si>
+  <si>
+    <t>Glurg Gift</t>
+  </si>
+  <si>
+    <t>Coins</t>
+  </si>
+  <si>
+    <t>Auto-Save Casino</t>
+  </si>
+  <si>
+    <t>Magmaclang</t>
+  </si>
+  <si>
+    <t>TN MSJ</t>
+  </si>
+  <si>
+    <t>Fred 4</t>
+  </si>
+  <si>
+    <t>Maxwell 2</t>
+  </si>
+  <si>
+    <t>Zurroaratr</t>
+  </si>
+  <si>
+    <t>Fishing Rod</t>
+  </si>
+  <si>
+    <t>Surf</t>
+  </si>
+  <si>
+    <t>Exp. Share</t>
+  </si>
+  <si>
+    <t>Lucky Egg</t>
+  </si>
+  <si>
+    <t>Rick 3</t>
+  </si>
+  <si>
+    <t>Triwandoliz</t>
+  </si>
+  <si>
+    <t>Diftery</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Grandma</t>
+  </si>
+  <si>
+    <t>1st Gate</t>
+  </si>
+  <si>
+    <t>Talk to Robin</t>
   </si>
 </sst>
 </file>
@@ -704,8 +834,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1040,16 +1173,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:C137"/>
+  <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="141.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,7 +1328,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1203,7 +1336,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1211,7 +1344,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1219,7 +1352,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1227,7 +1360,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1235,15 +1368,18 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1251,303 +1387,597 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>213</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24">
+        <v>7</v>
+      </c>
+      <c r="N24">
+        <v>8</v>
+      </c>
+      <c r="O24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>250</v>
+      </c>
+      <c r="G25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H25" t="s">
+        <v>252</v>
+      </c>
+      <c r="I25" t="s">
+        <v>214</v>
+      </c>
+      <c r="J25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>215</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>218</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>219</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>220</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>221</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>27</v>
+      </c>
+      <c r="D51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>31</v>
+      </c>
+      <c r="D55" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>34</v>
+      </c>
+      <c r="D58" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>35</v>
+      </c>
+      <c r="D59" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>36</v>
+      </c>
+      <c r="D60" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1555,7 +1985,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1563,7 +1993,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1571,7 +2001,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Redid horizontal gate, first split work for lab scripting and starters
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Microsoft\Excel\Pokemon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF132A83-5B4C-4510-A9B7-F535FF001517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70710DC2-7F9F-4DFF-9651-42C6F1FCEF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="260">
   <si>
     <t>Current</t>
   </si>
@@ -324,9 +323,6 @@
     <t>Gives Robin a short break, as thanks he goes back to the gym and allows you to fight him</t>
   </si>
   <si>
-    <t>Go back to post office, tell Robin you beat all the grunts and delivered all the packages: get Cut</t>
-  </si>
-  <si>
     <t>Load in, your dad is the professor, gives you your starter</t>
   </si>
   <si>
@@ -675,9 +671,6 @@
     <t>Afterwords, find some reason to go back to the lab to talk to your dad and get your dex upgraded for E pokemon</t>
   </si>
   <si>
-    <t>Post</t>
-  </si>
-  <si>
     <t>1st gate</t>
   </si>
   <si>
@@ -795,10 +788,34 @@
     <t>Grandma</t>
   </si>
   <si>
-    <t>1st Gate</t>
-  </si>
-  <si>
     <t>Talk to Robin</t>
+  </si>
+  <si>
+    <t>Give package to Warehouse owner, get Cut</t>
+  </si>
+  <si>
+    <t>Go back to post office, tell Robin you beat all the grunts and delivered all the packages</t>
+  </si>
+  <si>
+    <t>Go back to Robin, he gives you a 4th letter</t>
+  </si>
+  <si>
+    <t>Dad First</t>
+  </si>
+  <si>
+    <t>Pokedex 1</t>
+  </si>
+  <si>
+    <t># Badges</t>
+  </si>
+  <si>
+    <t>9 (Champ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once here, Dad will upgrade dex to </t>
+  </si>
+  <si>
+    <t>Gate 1</t>
   </si>
 </sst>
 </file>
@@ -834,10 +851,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:O137"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1212,10 +1232,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,7 +1243,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,10 +1251,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,10 +1262,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,7 +1273,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1271,6 +1291,9 @@
       <c r="B9" t="s">
         <v>83</v>
       </c>
+      <c r="C9" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1333,7 +1356,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1341,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1349,7 +1372,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1357,7 +1380,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1365,7 +1388,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1373,10 +1396,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1384,7 +1407,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1392,13 +1415,16 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="E24" t="s">
+        <v>256</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1436,31 +1462,37 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>254</v>
+      </c>
+      <c r="G25" t="s">
+        <v>248</v>
+      </c>
+      <c r="H25" t="s">
+        <v>255</v>
+      </c>
+      <c r="I25" t="s">
+        <v>249</v>
+      </c>
+      <c r="J25" t="s">
+        <v>259</v>
+      </c>
+      <c r="K25" t="s">
+        <v>212</v>
+      </c>
+      <c r="L25" t="s">
         <v>250</v>
-      </c>
-      <c r="G25" t="s">
-        <v>251</v>
-      </c>
-      <c r="H25" t="s">
-        <v>252</v>
-      </c>
-      <c r="I25" t="s">
-        <v>214</v>
-      </c>
-      <c r="J25" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1468,16 +1500,16 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1485,16 +1517,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1502,16 +1534,16 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1519,16 +1551,16 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1536,16 +1568,16 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C30">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1553,16 +1585,16 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C31">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E31">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -1570,16 +1602,16 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C32">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1587,16 +1619,16 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C33">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>222</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,13 +1636,16 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C34">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1618,13 +1653,13 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C35">
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,13 +1667,13 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,13 +1681,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1660,13 +1695,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,13 +1709,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C39">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,13 +1723,13 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="C40">
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,13 +1737,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C41">
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,13 +1751,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C42">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1730,13 +1765,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C43">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1744,13 +1779,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C44">
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,13 +1793,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C45">
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1772,13 +1807,13 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C46">
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,13 +1821,13 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C47">
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,13 +1835,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C48">
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1814,13 +1849,13 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C49">
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,13 +1863,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="C50">
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1842,13 +1877,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1856,13 +1891,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,13 +1905,13 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="C53">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,13 +1919,13 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C54">
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,13 +1933,13 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C55">
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,13 +1947,13 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C56">
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,13 +1961,13 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C57">
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,13 +1975,13 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,13 +1989,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1968,13 +2003,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C60">
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1982,7 +2017,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,7 +2025,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1998,7 +2033,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2006,7 +2041,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2057,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,7 +2065,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,7 +2073,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,7 +2081,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,7 +2089,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2062,7 +2097,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2070,7 +2105,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2078,7 +2113,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2086,7 +2121,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,7 +2129,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2102,7 +2137,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,7 +2145,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2118,7 +2153,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,7 +2161,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2134,7 +2169,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2177,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2150,285 +2185,295 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>180</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>164</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>70</v>
+        <v>167</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>203</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added vertical gate stuff and Avery part
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70710DC2-7F9F-4DFF-9651-42C6F1FCEF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54F0CAE-1537-4F4A-A816-DC83FC7D5591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -815,7 +815,7 @@
     <t xml:space="preserve">Once here, Dad will upgrade dex to </t>
   </si>
   <si>
-    <t>Gate 1</t>
+    <t>Avery</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished everything up to Poppy Grove!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54F0CAE-1537-4F4A-A816-DC83FC7D5591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391038EF-B51A-4CE3-BA36-B064200296B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -338,9 +338,6 @@
     <t>Scott is where he was before, you fight him, he gives you the item for your starter</t>
   </si>
   <si>
-    <t>If you go back to your dad, he gives you a second starter bc evil team is bad and hard</t>
-  </si>
-  <si>
     <t>You talk to Ryder for the first time, optionally, he gives Lv. 15 Abra</t>
   </si>
   <si>
@@ -816,6 +813,9 @@
   </si>
   <si>
     <t>Avery</t>
+  </si>
+  <si>
+    <t>Second Starter</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
         <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,7 +1292,7 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1388,18 +1388,15 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>100</v>
-      </c>
       <c r="C22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1407,7 +1404,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1421,10 +1418,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1468,31 +1465,34 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>253</v>
+      </c>
+      <c r="G25" t="s">
+        <v>247</v>
+      </c>
+      <c r="H25" t="s">
         <v>254</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>248</v>
       </c>
-      <c r="H25" t="s">
-        <v>255</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>258</v>
+      </c>
+      <c r="K25" t="s">
+        <v>211</v>
+      </c>
+      <c r="L25" t="s">
+        <v>259</v>
+      </c>
+      <c r="M25" t="s">
         <v>249</v>
-      </c>
-      <c r="J25" t="s">
-        <v>259</v>
-      </c>
-      <c r="K25" t="s">
-        <v>212</v>
-      </c>
-      <c r="L25" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1500,13 +1500,13 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1517,13 +1517,13 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1534,13 +1534,13 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1551,13 +1551,13 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1568,13 +1568,13 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1585,13 +1585,13 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -1602,13 +1602,13 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E32">
         <v>7</v>
@@ -1619,13 +1619,13 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
@@ -1636,16 +1636,16 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,13 +1653,13 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35">
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,13 +1667,13 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1681,13 +1681,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,13 +1709,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C39">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,13 +1737,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41">
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,13 +1751,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,13 +1765,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1779,13 +1779,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44">
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,13 +1793,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45">
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,13 +1807,13 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46">
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1821,13 +1821,13 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C47">
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1835,13 +1835,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C48">
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,13 +1849,13 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49">
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,13 +1863,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50">
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1877,13 +1877,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,13 +1919,13 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C54">
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,13 +1933,13 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C55">
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,13 +1947,13 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56">
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1961,13 +1961,13 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C57">
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,13 +1975,13 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1989,13 +1989,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,13 +2003,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C60">
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2049,7 +2049,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2105,7 +2105,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,7 +2121,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2145,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2153,7 +2153,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2161,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2169,7 +2169,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,55 +2190,55 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2248,32 +2248,32 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
@@ -2283,147 +2283,147 @@
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
@@ -2433,47 +2433,47 @@
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished story for gym 1 split!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391038EF-B51A-4CE3-BA36-B064200296B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBCB545-5701-45DA-B28D-ADC9509F4E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="267">
   <si>
     <t>Current</t>
   </si>
@@ -816,6 +816,27 @@
   </si>
   <si>
     <t>Second Starter</t>
+  </si>
+  <si>
+    <t>Tell Robin</t>
+  </si>
+  <si>
+    <t>Letter A</t>
+  </si>
+  <si>
+    <t>Letter B</t>
+  </si>
+  <si>
+    <t>Letter C</t>
+  </si>
+  <si>
+    <t>Letter D</t>
+  </si>
+  <si>
+    <t>WH Grunt</t>
+  </si>
+  <si>
+    <t>WH Unlock</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:O139"/>
+  <dimension ref="A1:Z139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1372,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1359,7 +1380,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1367,7 +1388,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1375,7 +1396,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1383,7 +1404,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1391,28 +1412,28 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1453,13 +1474,46 @@
       <c r="O24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>10</v>
+      </c>
+      <c r="Q24">
+        <v>11</v>
+      </c>
+      <c r="R24">
+        <v>12</v>
+      </c>
+      <c r="S24">
+        <v>13</v>
+      </c>
+      <c r="T24">
+        <v>14</v>
+      </c>
+      <c r="U24">
+        <v>15</v>
+      </c>
+      <c r="V24">
+        <v>16</v>
+      </c>
+      <c r="W24">
+        <v>17</v>
+      </c>
+      <c r="X24">
+        <v>18</v>
+      </c>
+      <c r="Y24">
+        <v>19</v>
+      </c>
+      <c r="Z24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1494,8 +1548,35 @@
       <c r="M25" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>261</v>
+      </c>
+      <c r="O25" t="s">
+        <v>262</v>
+      </c>
+      <c r="P25" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>260</v>
+      </c>
+      <c r="R25" t="s">
+        <v>265</v>
+      </c>
+      <c r="S25" t="s">
+        <v>266</v>
+      </c>
+      <c r="T25" t="s">
+        <v>212</v>
+      </c>
+      <c r="U25" t="s">
+        <v>264</v>
+      </c>
+      <c r="V25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1512,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1529,7 +1610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1546,7 +1627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1563,7 +1644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1580,7 +1661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1597,7 +1678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Work on maps for Gym 2 split
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBCB545-5701-45DA-B28D-ADC9509F4E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2D093E-5910-46B3-A9F3-A0B70ECC7FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="268">
   <si>
     <t>Current</t>
   </si>
@@ -837,6 +837,9 @@
   </si>
   <si>
     <t>WH Unlock</t>
+  </si>
+  <si>
+    <t>Crook</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1220,7 @@
   <dimension ref="A1:Z139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B24" sqref="B24:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,6 +1578,12 @@
       <c r="V25" t="s">
         <v>260</v>
       </c>
+      <c r="W25" t="s">
+        <v>267</v>
+      </c>
+      <c r="X25" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
Gym 2 split work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2D093E-5910-46B3-A9F3-A0B70ECC7FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA16D906-4D96-4345-B9F7-2D31321CD311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="271">
   <si>
     <t>Current</t>
   </si>
@@ -840,6 +840,15 @@
   </si>
   <si>
     <t>Crook</t>
+  </si>
+  <si>
+    <t>Fred 1</t>
+  </si>
+  <si>
+    <t>Researcher</t>
+  </si>
+  <si>
+    <t>Teleport</t>
   </si>
 </sst>
 </file>
@@ -1219,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:Z139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,6 +1610,15 @@
       <c r="E26">
         <v>1</v>
       </c>
+      <c r="F26" t="s">
+        <v>268</v>
+      </c>
+      <c r="G26" t="s">
+        <v>269</v>
+      </c>
+      <c r="H26" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
Gym 2 work and encounters redo
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EA259C-1775-4B37-BEBA-BF3BB0061146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804B5EEE-BD84-4076-BEA5-C1E9A2264D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="165" windowWidth="29040" windowHeight="15840" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="286">
   <si>
     <t>Current</t>
   </si>
@@ -1273,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:Z140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,6 +1706,9 @@
       <c r="V26" t="s">
         <v>275</v>
       </c>
+      <c r="W26" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
Finished Gym 2 split!!!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804B5EEE-BD84-4076-BEA5-C1E9A2264D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38718506-8C48-4DF5-BDB2-C8FEF11A7381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="165" windowWidth="29040" windowHeight="15840" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="286">
   <si>
     <t>Current</t>
   </si>
@@ -1274,7 +1274,7 @@
   <dimension ref="A1:Z140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,6 +1732,9 @@
       <c r="G27" t="s">
         <v>270</v>
       </c>
+      <c r="H27" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">

</xml_diff>

<commit_message>
New sprites and Gym 3 split work!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C64994-CEEA-45FD-9BFA-3F1DA76AA5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A530E39-78CC-4078-B069-A3CD391F2204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="165" windowWidth="29040" windowHeight="15840" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="297">
   <si>
     <t>Current</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Go to Mt. Splinkty and beat him, gives you Wire Cutters</t>
   </si>
   <si>
-    <t>Vine Cross HM on the floor in the room, go back and free Xurkitree</t>
-  </si>
-  <si>
     <t>Once you free him he goes ballistic, you have to beat him to calm him down, possessed trainers go away faster</t>
   </si>
   <si>
@@ -900,6 +897,36 @@
   </si>
   <si>
     <t>Regional</t>
+  </si>
+  <si>
+    <t>Millie 1</t>
+  </si>
+  <si>
+    <t>Millie 2</t>
+  </si>
+  <si>
+    <t>Chained Xurkitree</t>
+  </si>
+  <si>
+    <t>Millie 3</t>
+  </si>
+  <si>
+    <t>TN Splinkty</t>
+  </si>
+  <si>
+    <t>Free Xurkitree</t>
+  </si>
+  <si>
+    <t>UP Xurkitree</t>
+  </si>
+  <si>
+    <t>Millie 4</t>
+  </si>
+  <si>
+    <t>She gives you Vine Cross and gets out of your way, free Xurkitree</t>
+  </si>
+  <si>
+    <t>Go back to Kleine and talk to Millie blocking the way saying she was holding off the possessed ppl for you</t>
   </si>
 </sst>
 </file>
@@ -1277,19 +1304,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:Z140"/>
+  <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.7109375" customWidth="1"/>
+    <col min="2" max="2" width="93.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1327,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1308,10 +1335,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1319,10 +1346,10 @@
         <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1330,7 +1357,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1338,10 +1365,10 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1349,10 +1376,10 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1387,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1376,10 +1403,10 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1387,7 +1414,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1395,7 +1422,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1403,7 +1430,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +1438,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1446,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1427,7 +1454,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1435,15 +1462,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1451,7 +1478,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1459,7 +1486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1467,23 +1494,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1491,7 +1518,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1502,10 +1529,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1571,81 +1598,81 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" t="s">
+        <v>243</v>
+      </c>
+      <c r="H25" t="s">
         <v>250</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>244</v>
       </c>
-      <c r="H25" t="s">
-        <v>251</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>254</v>
+      </c>
+      <c r="K25" t="s">
+        <v>207</v>
+      </c>
+      <c r="L25" t="s">
+        <v>255</v>
+      </c>
+      <c r="M25" t="s">
         <v>245</v>
       </c>
-      <c r="J25" t="s">
-        <v>255</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="N25" t="s">
+        <v>257</v>
+      </c>
+      <c r="O25" t="s">
+        <v>258</v>
+      </c>
+      <c r="P25" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>256</v>
+      </c>
+      <c r="R25" t="s">
+        <v>261</v>
+      </c>
+      <c r="S25" t="s">
+        <v>262</v>
+      </c>
+      <c r="T25" t="s">
         <v>208</v>
       </c>
-      <c r="L25" t="s">
+      <c r="U25" t="s">
+        <v>260</v>
+      </c>
+      <c r="V25" t="s">
         <v>256</v>
       </c>
-      <c r="M25" t="s">
-        <v>246</v>
-      </c>
-      <c r="N25" t="s">
-        <v>258</v>
-      </c>
-      <c r="O25" t="s">
-        <v>259</v>
-      </c>
-      <c r="P25" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>257</v>
-      </c>
-      <c r="R25" t="s">
-        <v>262</v>
-      </c>
-      <c r="S25" t="s">
+      <c r="W25" t="s">
         <v>263</v>
       </c>
-      <c r="T25" t="s">
-        <v>209</v>
-      </c>
-      <c r="U25" t="s">
-        <v>261</v>
-      </c>
-      <c r="V25" t="s">
-        <v>257</v>
-      </c>
-      <c r="W25" t="s">
-        <v>264</v>
-      </c>
       <c r="X25" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1656,70 +1683,70 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G26" t="s">
         <v>265</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>266</v>
       </c>
-      <c r="H26" t="s">
-        <v>267</v>
-      </c>
       <c r="I26" t="s">
+        <v>270</v>
+      </c>
+      <c r="J26" t="s">
+        <v>282</v>
+      </c>
+      <c r="K26" t="s">
+        <v>277</v>
+      </c>
+      <c r="L26" t="s">
         <v>271</v>
       </c>
-      <c r="J26" t="s">
-        <v>283</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
+        <v>276</v>
+      </c>
+      <c r="N26" t="s">
+        <v>272</v>
+      </c>
+      <c r="O26" t="s">
+        <v>274</v>
+      </c>
+      <c r="P26" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q26" t="s">
         <v>278</v>
       </c>
-      <c r="L26" t="s">
-        <v>272</v>
-      </c>
-      <c r="M26" t="s">
-        <v>277</v>
-      </c>
-      <c r="N26" t="s">
-        <v>273</v>
-      </c>
-      <c r="O26" t="s">
+      <c r="R26" t="s">
         <v>275</v>
       </c>
-      <c r="P26" t="s">
+      <c r="S26" t="s">
+        <v>279</v>
+      </c>
+      <c r="T26" t="s">
+        <v>280</v>
+      </c>
+      <c r="U26" t="s">
+        <v>281</v>
+      </c>
+      <c r="V26" t="s">
         <v>274</v>
       </c>
-      <c r="Q26" t="s">
-        <v>279</v>
-      </c>
-      <c r="R26" t="s">
-        <v>276</v>
-      </c>
-      <c r="S26" t="s">
-        <v>280</v>
-      </c>
-      <c r="T26" t="s">
-        <v>281</v>
-      </c>
-      <c r="U26" t="s">
-        <v>282</v>
-      </c>
-      <c r="V26" t="s">
-        <v>275</v>
-      </c>
       <c r="W26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X26" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1730,25 +1757,52 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>210</v>
+      </c>
+      <c r="G27" t="s">
+        <v>269</v>
+      </c>
+      <c r="H27" t="s">
+        <v>218</v>
+      </c>
+      <c r="I27" t="s">
+        <v>286</v>
+      </c>
+      <c r="J27" t="s">
+        <v>287</v>
+      </c>
+      <c r="K27" t="s">
+        <v>288</v>
+      </c>
+      <c r="L27" t="s">
         <v>211</v>
       </c>
-      <c r="G27" t="s">
-        <v>270</v>
-      </c>
-      <c r="H27" t="s">
-        <v>219</v>
-      </c>
-      <c r="I27" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>289</v>
+      </c>
+      <c r="N27" t="s">
+        <v>290</v>
+      </c>
+      <c r="O27" t="s">
+        <v>291</v>
+      </c>
+      <c r="P27" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>293</v>
+      </c>
+      <c r="R27" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1759,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1776,13 +1830,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1793,13 +1847,13 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1810,13 +1864,13 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E31">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1827,13 +1881,13 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1844,13 +1898,13 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1861,13 +1915,13 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1878,10 +1932,10 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1892,38 +1946,38 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1934,10 +1988,10 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1948,10 +2002,10 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1962,10 +2016,10 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1976,10 +2030,10 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1990,10 +2044,10 @@
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2004,10 +2058,10 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2018,10 +2072,10 @@
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2032,10 +2086,10 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2046,10 +2100,10 @@
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2060,10 +2114,10 @@
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2074,10 +2128,10 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2088,616 +2142,621 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>296</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>295</v>
       </c>
       <c r="C52">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="C53">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C54">
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>32</v>
       </c>
       <c r="C55">
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C56">
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C57">
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C60">
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>149</v>
+      </c>
+      <c r="C85" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>176</v>
-      </c>
-      <c r="C85" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated trainers and bug fixes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6497747-CF54-4DA5-AC1C-5AB0413B48EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0EE78-3850-487D-911F-513858178A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="28680" yWindow="-12660" windowWidth="16440" windowHeight="28320" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="297">
   <si>
     <t>Current</t>
   </si>
@@ -377,9 +377,6 @@
     <t>Go north to Route 26, fight Scott 2 (north of Timburr trainer)</t>
   </si>
   <si>
-    <t>Add spots for Dex Nav and Ability Patches</t>
-  </si>
-  <si>
     <t>Get to Kleine, Millie says that trainers are possessed, a bunch of (optional) trainers outside</t>
   </si>
   <si>
@@ -797,9 +794,6 @@
     <t>9 (Champ)</t>
   </si>
   <si>
-    <t xml:space="preserve">Once here, Dad will upgrade dex to </t>
-  </si>
-  <si>
     <t>Avery</t>
   </si>
   <si>
@@ -930,6 +924,9 @@
   </si>
   <si>
     <t>Millie 5</t>
+  </si>
+  <si>
+    <t>ADD RAZOR CLAW IN CROSSABLE BRIDGE ON ROUTE 45 NEAR PHOTON'S RESEARCH CENTER</t>
   </si>
 </sst>
 </file>
@@ -1309,17 +1306,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.6640625" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1327,10 +1324,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1338,10 +1335,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1349,10 +1346,10 @@
         <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1357,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1368,10 +1365,10 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1379,10 +1376,10 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1398,18 +1395,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1411,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1425,7 +1419,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1433,7 +1427,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1441,7 +1435,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1457,7 +1451,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1465,15 +1459,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1481,7 +1475,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1489,7 +1483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1497,23 +1491,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1515,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1532,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1601,81 +1595,81 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>248</v>
+      </c>
+      <c r="G25" t="s">
+        <v>242</v>
+      </c>
+      <c r="H25" t="s">
         <v>249</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>243</v>
       </c>
-      <c r="H25" t="s">
-        <v>250</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>252</v>
+      </c>
+      <c r="K25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L25" t="s">
+        <v>253</v>
+      </c>
+      <c r="M25" t="s">
         <v>244</v>
       </c>
-      <c r="J25" t="s">
+      <c r="N25" t="s">
+        <v>255</v>
+      </c>
+      <c r="O25" t="s">
+        <v>256</v>
+      </c>
+      <c r="P25" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q25" t="s">
         <v>254</v>
       </c>
-      <c r="K25" t="s">
+      <c r="R25" t="s">
+        <v>259</v>
+      </c>
+      <c r="S25" t="s">
+        <v>260</v>
+      </c>
+      <c r="T25" t="s">
         <v>207</v>
       </c>
-      <c r="L25" t="s">
-        <v>255</v>
-      </c>
-      <c r="M25" t="s">
-        <v>245</v>
-      </c>
-      <c r="N25" t="s">
-        <v>257</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="U25" t="s">
         <v>258</v>
       </c>
-      <c r="P25" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>256</v>
-      </c>
-      <c r="R25" t="s">
+      <c r="V25" t="s">
+        <v>254</v>
+      </c>
+      <c r="W25" t="s">
         <v>261</v>
       </c>
-      <c r="S25" t="s">
-        <v>262</v>
-      </c>
-      <c r="T25" t="s">
-        <v>208</v>
-      </c>
-      <c r="U25" t="s">
-        <v>260</v>
-      </c>
-      <c r="V25" t="s">
-        <v>256</v>
-      </c>
-      <c r="W25" t="s">
-        <v>263</v>
-      </c>
       <c r="X25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1686,70 +1680,70 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>262</v>
+      </c>
+      <c r="G26" t="s">
+        <v>263</v>
+      </c>
+      <c r="H26" t="s">
         <v>264</v>
       </c>
-      <c r="G26" t="s">
-        <v>265</v>
-      </c>
-      <c r="H26" t="s">
-        <v>266</v>
-      </c>
       <c r="I26" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" t="s">
+        <v>280</v>
+      </c>
+      <c r="K26" t="s">
+        <v>275</v>
+      </c>
+      <c r="L26" t="s">
+        <v>269</v>
+      </c>
+      <c r="M26" t="s">
+        <v>274</v>
+      </c>
+      <c r="N26" t="s">
         <v>270</v>
       </c>
-      <c r="J26" t="s">
-        <v>282</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="O26" t="s">
+        <v>272</v>
+      </c>
+      <c r="P26" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>276</v>
+      </c>
+      <c r="R26" t="s">
+        <v>273</v>
+      </c>
+      <c r="S26" t="s">
         <v>277</v>
       </c>
-      <c r="L26" t="s">
-        <v>271</v>
-      </c>
-      <c r="M26" t="s">
-        <v>276</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="T26" t="s">
+        <v>278</v>
+      </c>
+      <c r="U26" t="s">
+        <v>279</v>
+      </c>
+      <c r="V26" t="s">
         <v>272</v>
       </c>
-      <c r="O26" t="s">
-        <v>274</v>
-      </c>
-      <c r="P26" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>278</v>
-      </c>
-      <c r="R26" t="s">
-        <v>275</v>
-      </c>
-      <c r="S26" t="s">
-        <v>279</v>
-      </c>
-      <c r="T26" t="s">
-        <v>280</v>
-      </c>
-      <c r="U26" t="s">
-        <v>281</v>
-      </c>
-      <c r="V26" t="s">
-        <v>274</v>
-      </c>
       <c r="W26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X26" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1760,55 +1754,55 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27" t="s">
+        <v>267</v>
+      </c>
+      <c r="H27" t="s">
+        <v>217</v>
+      </c>
+      <c r="I27" t="s">
+        <v>284</v>
+      </c>
+      <c r="J27" t="s">
+        <v>285</v>
+      </c>
+      <c r="K27" t="s">
+        <v>286</v>
+      </c>
+      <c r="L27" t="s">
         <v>210</v>
       </c>
-      <c r="G27" t="s">
-        <v>269</v>
-      </c>
-      <c r="H27" t="s">
-        <v>218</v>
-      </c>
-      <c r="I27" t="s">
-        <v>286</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="M27" t="s">
         <v>287</v>
       </c>
-      <c r="K27" t="s">
+      <c r="N27" t="s">
         <v>288</v>
       </c>
-      <c r="L27" t="s">
-        <v>211</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>289</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q27" t="s">
         <v>290</v>
       </c>
-      <c r="O27" t="s">
+      <c r="R27" t="s">
         <v>291</v>
       </c>
-      <c r="P27" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>292</v>
-      </c>
-      <c r="R27" t="s">
-        <v>293</v>
-      </c>
       <c r="S27" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1819,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1836,13 +1830,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1853,13 +1847,13 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1870,13 +1864,13 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E31">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1887,13 +1881,13 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1904,13 +1898,13 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1921,13 +1915,13 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1938,10 +1932,10 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1952,38 +1946,38 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1994,10 +1988,10 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2008,10 +2002,10 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2022,10 +2016,10 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2036,164 +2030,164 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44">
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C45">
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46">
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47">
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48">
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49">
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50">
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C52">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2204,10 +2198,10 @@
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2218,160 +2212,160 @@
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C56">
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C57">
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C60">
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2379,7 +2373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2387,382 +2381,382 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
+        <v>148</v>
+      </c>
+      <c r="C85" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>149</v>
       </c>
-      <c r="C85" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B92" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B93" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B101" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B105" t="s">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B106" t="s">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B107" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B108" t="s">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B109" t="s">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B110" t="s">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B112" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B113" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B114" t="s">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B115" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B116" t="s">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B117" t="s">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B118" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B119" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B121" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B122" t="s">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B129" t="s">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B130" t="s">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B131" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B134" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B135" t="s">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B136" t="s">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B137" t="s">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B138" t="s">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B139" t="s">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B140" t="s">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B141" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Gym 3 split (except for Gym Trainers + Leader levels)!!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0EE78-3850-487D-911F-513858178A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA8A60-16D5-403A-8658-6C64748A252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12660" windowWidth="16440" windowHeight="28320" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="296">
   <si>
     <t>Current</t>
   </si>
@@ -921,9 +921,6 @@
   </si>
   <si>
     <t>Go back to Kleine and talk to Millie blocking the way saying she was holding off the possessed ppl for you</t>
-  </si>
-  <si>
-    <t>Millie 5</t>
   </si>
   <si>
     <t>ADD RAZOR CLAW IN CROSSABLE BRIDGE ON ROUTE 45 NEAR PHOTON'S RESEARCH CENTER</t>
@@ -1306,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1797,9 +1794,6 @@
       </c>
       <c r="R27" t="s">
         <v>291</v>
-      </c>
-      <c r="S27" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed to work with Java 8, bug fixes and level curve work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DFB74C-FE7F-4112-9607-172AE2E6F25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C7EC1-117B-48FD-B0F4-A1988D82AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="310">
   <si>
     <t>Current</t>
   </si>
@@ -410,12 +410,6 @@
     <t>Arrive at Schrice City, weird rainbows and glowy stuff on the screen (use UI class?)</t>
   </si>
   <si>
-    <t>Hurts to go outside, it's so bright and warped and weird, add npc that is blind and gives you visor</t>
-  </si>
-  <si>
-    <t>In the Pokemon Center, crowded with people (?), Ryder is in there</t>
-  </si>
-  <si>
     <t>Ryder says he just pulled up, it's bright as hell, explains what is happening and gives you a Flamigo which should help</t>
   </si>
   <si>
@@ -927,6 +921,51 @@
   </si>
   <si>
     <t>Millie 5</t>
+  </si>
+  <si>
+    <t>Gift fossil</t>
+  </si>
+  <si>
+    <t>Ryder 3</t>
+  </si>
+  <si>
+    <t>Hurts to go outside, it's so bright and warped and weird</t>
+  </si>
+  <si>
+    <t>In the Pokemon Center, crowded with people (?), Ryder is in there, gives you visor</t>
+  </si>
+  <si>
+    <t>Ice Master</t>
+  </si>
+  <si>
+    <t>Ground Master</t>
+  </si>
+  <si>
+    <t>G Unlock</t>
+  </si>
+  <si>
+    <t>I Unlock</t>
+  </si>
+  <si>
+    <t>Shovel</t>
+  </si>
+  <si>
+    <t>Ice Pick</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>UP Cairnasaur</t>
+  </si>
+  <si>
+    <t>Gym 4</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>UP Shookwat</t>
   </si>
 </sst>
 </file>
@@ -1306,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1335,7 +1374,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,7 +1385,7 @@
         <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1365,7 +1404,7 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1415,7 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,7 +1503,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -1496,7 +1535,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -1504,7 +1543,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1526,10 +1565,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1600,73 +1639,73 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G25" t="s">
+        <v>240</v>
+      </c>
+      <c r="H25" t="s">
+        <v>247</v>
+      </c>
+      <c r="I25" t="s">
+        <v>241</v>
+      </c>
+      <c r="J25" t="s">
+        <v>250</v>
+      </c>
+      <c r="K25" t="s">
+        <v>204</v>
+      </c>
+      <c r="L25" t="s">
+        <v>251</v>
+      </c>
+      <c r="M25" t="s">
         <v>242</v>
       </c>
-      <c r="H25" t="s">
-        <v>249</v>
-      </c>
-      <c r="I25" t="s">
-        <v>243</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="N25" t="s">
+        <v>253</v>
+      </c>
+      <c r="O25" t="s">
+        <v>254</v>
+      </c>
+      <c r="P25" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q25" t="s">
         <v>252</v>
       </c>
-      <c r="K25" t="s">
-        <v>206</v>
-      </c>
-      <c r="L25" t="s">
-        <v>253</v>
-      </c>
-      <c r="M25" t="s">
-        <v>244</v>
-      </c>
-      <c r="N25" t="s">
-        <v>255</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="R25" t="s">
+        <v>257</v>
+      </c>
+      <c r="S25" t="s">
+        <v>258</v>
+      </c>
+      <c r="T25" t="s">
+        <v>205</v>
+      </c>
+      <c r="U25" t="s">
         <v>256</v>
       </c>
-      <c r="P25" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>254</v>
-      </c>
-      <c r="R25" t="s">
+      <c r="V25" t="s">
+        <v>252</v>
+      </c>
+      <c r="W25" t="s">
         <v>259</v>
       </c>
-      <c r="S25" t="s">
-        <v>260</v>
-      </c>
-      <c r="T25" t="s">
-        <v>207</v>
-      </c>
-      <c r="U25" t="s">
-        <v>258</v>
-      </c>
-      <c r="V25" t="s">
-        <v>254</v>
-      </c>
-      <c r="W25" t="s">
-        <v>261</v>
-      </c>
       <c r="X25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1680,67 +1719,67 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G26" t="s">
+        <v>261</v>
+      </c>
+      <c r="H26" t="s">
         <v>262</v>
       </c>
-      <c r="G26" t="s">
-        <v>263</v>
-      </c>
-      <c r="H26" t="s">
-        <v>264</v>
-      </c>
       <c r="I26" t="s">
+        <v>266</v>
+      </c>
+      <c r="J26" t="s">
+        <v>278</v>
+      </c>
+      <c r="K26" t="s">
+        <v>273</v>
+      </c>
+      <c r="L26" t="s">
+        <v>267</v>
+      </c>
+      <c r="M26" t="s">
+        <v>272</v>
+      </c>
+      <c r="N26" t="s">
         <v>268</v>
       </c>
-      <c r="J26" t="s">
-        <v>280</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="O26" t="s">
+        <v>270</v>
+      </c>
+      <c r="P26" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>274</v>
+      </c>
+      <c r="R26" t="s">
+        <v>271</v>
+      </c>
+      <c r="S26" t="s">
         <v>275</v>
       </c>
-      <c r="L26" t="s">
-        <v>269</v>
-      </c>
-      <c r="M26" t="s">
-        <v>274</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="T26" t="s">
+        <v>276</v>
+      </c>
+      <c r="U26" t="s">
+        <v>277</v>
+      </c>
+      <c r="V26" t="s">
         <v>270</v>
       </c>
-      <c r="O26" t="s">
-        <v>272</v>
-      </c>
-      <c r="P26" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>276</v>
-      </c>
-      <c r="R26" t="s">
-        <v>273</v>
-      </c>
-      <c r="S26" t="s">
-        <v>277</v>
-      </c>
-      <c r="T26" t="s">
-        <v>278</v>
-      </c>
-      <c r="U26" t="s">
-        <v>279</v>
-      </c>
-      <c r="V26" t="s">
-        <v>272</v>
-      </c>
       <c r="W26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="X26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1754,52 +1793,55 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I27" t="s">
+        <v>282</v>
+      </c>
+      <c r="J27" t="s">
+        <v>283</v>
+      </c>
+      <c r="K27" t="s">
         <v>284</v>
       </c>
-      <c r="J27" t="s">
+      <c r="L27" t="s">
+        <v>208</v>
+      </c>
+      <c r="M27" t="s">
         <v>285</v>
       </c>
-      <c r="K27" t="s">
+      <c r="N27" t="s">
         <v>286</v>
       </c>
-      <c r="L27" t="s">
-        <v>210</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>287</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q27" t="s">
         <v>288</v>
       </c>
-      <c r="O27" t="s">
+      <c r="R27" t="s">
         <v>289</v>
       </c>
-      <c r="P27" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>290</v>
-      </c>
-      <c r="R27" t="s">
-        <v>291</v>
-      </c>
       <c r="S27" t="s">
-        <v>296</v>
+        <v>294</v>
+      </c>
+      <c r="T27" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1813,10 +1855,43 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E28">
         <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>296</v>
+      </c>
+      <c r="G28" t="s">
+        <v>299</v>
+      </c>
+      <c r="H28" t="s">
+        <v>300</v>
+      </c>
+      <c r="I28" t="s">
+        <v>302</v>
+      </c>
+      <c r="J28" t="s">
+        <v>301</v>
+      </c>
+      <c r="K28" t="s">
+        <v>303</v>
+      </c>
+      <c r="L28" t="s">
+        <v>304</v>
+      </c>
+      <c r="M28" t="s">
+        <v>305</v>
+      </c>
+      <c r="N28" t="s">
+        <v>306</v>
+      </c>
+      <c r="O28" t="s">
+        <v>217</v>
+      </c>
+      <c r="P28" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -1830,10 +1905,28 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E29">
         <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>308</v>
+      </c>
+      <c r="G29" t="s">
+        <v>218</v>
+      </c>
+      <c r="H29" t="s">
+        <v>219</v>
+      </c>
+      <c r="I29" t="s">
+        <v>309</v>
+      </c>
+      <c r="J29" t="s">
+        <v>221</v>
+      </c>
+      <c r="K29" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1847,7 +1940,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1864,7 +1957,7 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -1881,7 +1974,7 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E32">
         <v>7</v>
@@ -1898,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
@@ -1915,10 +2008,10 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1932,7 +2025,7 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1946,7 +2039,7 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1954,13 +2047,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1968,13 +2061,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,7 +2081,7 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2002,7 +2095,7 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2016,7 +2109,7 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2030,7 +2123,7 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2044,7 +2137,7 @@
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2151,7 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,7 +2165,7 @@
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2086,7 +2179,7 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2100,7 +2193,7 @@
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,7 +2207,7 @@
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,7 +2221,7 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2235,7 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2150,13 +2243,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,13 +2257,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C52">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,7 +2277,7 @@
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,7 +2291,7 @@
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,7 +2305,7 @@
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,7 +2319,7 @@
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,7 +2333,7 @@
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2248,13 +2341,13 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>297</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2262,13 +2355,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>298</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2276,13 +2369,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60">
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2290,7 +2383,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,7 +2391,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2306,7 +2399,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,7 +2407,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2322,7 +2415,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2330,7 +2423,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2338,7 +2431,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2346,7 +2439,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2354,7 +2447,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2362,7 +2455,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2386,7 +2479,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2394,7 +2487,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2402,7 +2495,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2410,7 +2503,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2418,7 +2511,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2426,7 +2519,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2434,7 +2527,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2442,7 +2535,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2450,7 +2543,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2458,7 +2551,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2473,55 +2566,55 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C85" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2531,32 +2624,32 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
@@ -2566,147 +2659,147 @@
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
@@ -2716,47 +2809,47 @@
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a couple more trainer classes and refactored block setup
to account for all directions
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C7EC1-117B-48FD-B0F4-A1988D82AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE5FFD9-0130-4AAD-8ADC-37FE2A2426D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -947,12 +947,6 @@
     <t>I Unlock</t>
   </si>
   <si>
-    <t>Shovel</t>
-  </si>
-  <si>
-    <t>Ice Pick</t>
-  </si>
-  <si>
     <t>Principal</t>
   </si>
   <si>
@@ -966,6 +960,12 @@
   </si>
   <si>
     <t>UP Shookwat</t>
+  </si>
+  <si>
+    <t>I Clear</t>
+  </si>
+  <si>
+    <t>G Clear</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,22 +1876,22 @@
         <v>301</v>
       </c>
       <c r="K28" t="s">
+        <v>308</v>
+      </c>
+      <c r="L28" t="s">
+        <v>309</v>
+      </c>
+      <c r="M28" t="s">
         <v>303</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>304</v>
-      </c>
-      <c r="M28" t="s">
-        <v>305</v>
-      </c>
-      <c r="N28" t="s">
-        <v>306</v>
       </c>
       <c r="O28" t="s">
         <v>217</v>
       </c>
       <c r="P28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G29" t="s">
         <v>218</v>
@@ -1920,7 +1920,7 @@
         <v>219</v>
       </c>
       <c r="I29" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J29" t="s">
         <v>221</v>

</xml_diff>

<commit_message>
Added spinning trainers 1-3 split, and gym 4 split work!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE5FFD9-0130-4AAD-8ADC-37FE2A2426D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56681778-A17A-496D-9289-1B398846B91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="312">
   <si>
     <t>Current</t>
   </si>
@@ -966,6 +966,12 @@
   </si>
   <si>
     <t>G Clear</t>
+  </si>
+  <si>
+    <t>Petticoat</t>
+  </si>
+  <si>
+    <t>Valiant</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1352,7 @@
   <dimension ref="A1:Z141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,6 +1897,12 @@
         <v>217</v>
       </c>
       <c r="P28" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>311</v>
+      </c>
+      <c r="R28" t="s">
         <v>305</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Redid player and tile drawing, bug fixes, and added ERM's berries
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56681778-A17A-496D-9289-1B398846B91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF917CD-B1DA-4237-9935-9B2D934011BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="317">
   <si>
     <t>Current</t>
   </si>
@@ -972,6 +972,21 @@
   </si>
   <si>
     <t>Valiant</t>
+  </si>
+  <si>
+    <t>1 in R23 maze from left side, 1 in R42 maze from right side</t>
+  </si>
+  <si>
+    <t>1 in heart of R23 maze, 1 in R45 past Psychic</t>
+  </si>
+  <si>
+    <t>1 in cell park</t>
+  </si>
+  <si>
+    <t>1 R29 past vine cross by dawn stone and gold bottle cap</t>
+  </si>
+  <si>
+    <t>1 in Gym 6+ past berry shop</t>
   </si>
 </sst>
 </file>
@@ -1349,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:Z141"/>
+  <dimension ref="A1:AA141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="AA30" sqref="AA30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1519,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1512,7 +1527,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1520,7 +1535,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1528,7 +1543,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1536,7 +1551,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1544,7 +1559,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1552,7 +1567,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1560,7 +1575,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1640,7 +1655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1713,8 +1728,11 @@
       <c r="X25" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1787,8 +1805,11 @@
       <c r="X26" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1849,8 +1870,11 @@
       <c r="T27" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA27" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1905,8 +1929,11 @@
       <c r="R28" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA28" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1940,8 +1967,11 @@
       <c r="K29" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA29" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1958,7 +1988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1975,7 +2005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Gym 4 maps and dialogue done!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF917CD-B1DA-4237-9935-9B2D934011BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB996E1-70E7-416D-A690-1A3D89AC5933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="317">
   <si>
     <t>Current</t>
   </si>
@@ -1366,14 +1366,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="AA30" sqref="AA30"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="AB37" sqref="AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.7109375" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fixes, dialogue additions, and playtested a bit
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB996E1-70E7-416D-A690-1A3D89AC5933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B80A69-0930-4F31-8B19-D4222A35ABCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -1366,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="AB37" sqref="AB37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Lots of bug fixes and gym 6 work!!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D16A3-6128-439A-AD3D-66C76754C8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6166E6CA-282E-4920-93B0-632695FF4F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12660" windowWidth="16440" windowHeight="28320" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="328">
   <si>
     <t>Current</t>
   </si>
@@ -1017,6 +1017,9 @@
   </si>
   <si>
     <t>Merlin explains how one is logic and one is faith and then asks you which you think will stop Dragowrath: logic or faith</t>
+  </si>
+  <si>
+    <t>Arthra Talk</t>
   </si>
 </sst>
 </file>
@@ -1396,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,24 +2024,27 @@
         <v>316</v>
       </c>
       <c r="G30" t="s">
+        <v>327</v>
+      </c>
+      <c r="H30" t="s">
         <v>221</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>317</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>222</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>318</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>223</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>224</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>319</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gym 6 scripting and gym work!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9A4333-7DA2-4DD6-8FEC-AC2863D03788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474DE60B-5D78-4083-86C3-4175F0CEEE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="329">
   <si>
     <t>Current</t>
   </si>
@@ -1020,6 +1020,9 @@
   </si>
   <si>
     <t>Arthra Talk</t>
+  </si>
+  <si>
+    <t>Maxwell After</t>
   </si>
 </sst>
 </file>
@@ -1399,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,6 +2050,9 @@
       <c r="N30" t="s">
         <v>319</v>
       </c>
+      <c r="O30" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">

</xml_diff>

<commit_message>
Gym 6 trainers, Gym 7 split casino and scripting work!!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474DE60B-5D78-4083-86C3-4175F0CEEE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68759DE3-DB10-42DC-AB69-DE0546749653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -998,9 +998,6 @@
     <t>Gym 6</t>
   </si>
   <si>
-    <t>If you didn't pick up Whirlpool he tells you where it is</t>
-  </si>
-  <si>
     <t>Scott Scene</t>
   </si>
   <si>
@@ -1023,6 +1020,9 @@
   </si>
   <si>
     <t>Maxwell After</t>
+  </si>
+  <si>
+    <t>If you didn't pick up Whirlpool he tells you where it is (he talked to Fred, and even tho he's resentful for joining Eclipse he still tried to help you guys)</t>
   </si>
 </sst>
 </file>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2027,7 @@
         <v>316</v>
       </c>
       <c r="G30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H30" t="s">
         <v>221</v>
@@ -2051,7 +2051,7 @@
         <v>319</v>
       </c>
       <c r="O30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
@@ -2071,25 +2071,25 @@
         <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G31" t="s">
         <v>225</v>
       </c>
       <c r="H31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I31" t="s">
         <v>227</v>
       </c>
       <c r="J31" t="s">
+        <v>322</v>
+      </c>
+      <c r="K31" t="s">
         <v>323</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>324</v>
-      </c>
-      <c r="L31" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A TON of changes over the course of the cruise week!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3360E822-92F9-4965-B5D0-AAC126627F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3EAD8-FAFE-4710-AFDB-383F7B75FDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12660" windowWidth="16440" windowHeight="28320" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="357">
   <si>
     <t>Current</t>
   </si>
@@ -473,9 +473,6 @@
     <t>Add starters base forms obtainable in a repeatable way</t>
   </si>
   <si>
-    <t>Update prize shop, make prize mons available multiple times and it costs your win streak or something</t>
-  </si>
-  <si>
     <t>Reach Ghostly Woods, lots of Ghosts swarming from UP Pheromosa powering a ghost machine to power up ghosts</t>
   </si>
   <si>
@@ -827,9 +824,6 @@
     <t>Ice Master teaches class on enduring the wild, Ground Master teaches class on digging (related to digging duo)</t>
   </si>
   <si>
-    <t>Access Checkpoint Charlie (Leviathan League), fight the elite four, who are  1) Whiskeroar, 2) Ryder's girlfriend (Poison), 3) Ground Master, 4) Arthra (Steel)</t>
-  </si>
-  <si>
     <t>Ryder 2</t>
   </si>
   <si>
@@ -1026,6 +1020,93 @@
   </si>
   <si>
     <t>Photon Gift</t>
+  </si>
+  <si>
+    <t>Access Checkpoint Charlie (Leviathan League), fight the elite four, who are  1) Whiskeroar, 2) Ryder's girlfriend (Poison), 3) Mom (Ground), 4) Arthra (Steel)</t>
+  </si>
+  <si>
+    <t>Arthra Scene</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Drago S1</t>
+  </si>
+  <si>
+    <t>UP Pheromosa</t>
+  </si>
+  <si>
+    <t>Dis Machine</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>Faith</t>
+  </si>
+  <si>
+    <t>Awake</t>
+  </si>
+  <si>
+    <t>Relomidel</t>
+  </si>
+  <si>
+    <t>Relopamil</t>
+  </si>
+  <si>
+    <t>Drago S2</t>
+  </si>
+  <si>
+    <t>Ryder Shack</t>
+  </si>
+  <si>
+    <t>Ryder Pos</t>
+  </si>
+  <si>
+    <t>Get in Ship</t>
+  </si>
+  <si>
+    <t>Arthra Space</t>
+  </si>
+  <si>
+    <t>Dragowrath</t>
+  </si>
+  <si>
+    <t>Nova Scene</t>
+  </si>
+  <si>
+    <t>Gym 8</t>
+  </si>
+  <si>
+    <t>Nova Ship</t>
+  </si>
+  <si>
+    <t>Robin Letter</t>
+  </si>
+  <si>
+    <t>Dad Scene</t>
+  </si>
+  <si>
+    <t>Scott 5</t>
+  </si>
+  <si>
+    <t>Fred 5</t>
+  </si>
+  <si>
+    <t>Fighting E4</t>
+  </si>
+  <si>
+    <t>Poison E4</t>
+  </si>
+  <si>
+    <t>Ground E4</t>
+  </si>
+  <si>
+    <t>Steel E4</t>
+  </si>
+  <si>
+    <t>Champion</t>
   </si>
 </sst>
 </file>
@@ -1405,17 +1486,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.7109375" customWidth="1"/>
+    <col min="2" max="2" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1423,10 +1504,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1437,18 +1518,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
       </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1456,7 +1534,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1464,10 +1542,10 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1475,10 +1553,10 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1564,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1494,7 +1572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1502,7 +1580,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1588,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1518,7 +1596,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1526,7 +1604,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1534,7 +1612,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1542,7 +1620,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1550,7 +1628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1558,15 +1636,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1574,7 +1652,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1582,7 +1660,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1590,23 +1668,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1614,7 +1692,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1625,10 +1703,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1694,84 +1772,84 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>244</v>
+      </c>
+      <c r="G25" t="s">
+        <v>238</v>
+      </c>
+      <c r="H25" t="s">
         <v>245</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>239</v>
       </c>
-      <c r="H25" t="s">
-        <v>246</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>248</v>
+      </c>
+      <c r="K25" t="s">
+        <v>202</v>
+      </c>
+      <c r="L25" t="s">
+        <v>249</v>
+      </c>
+      <c r="M25" t="s">
         <v>240</v>
       </c>
-      <c r="J25" t="s">
-        <v>249</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="N25" t="s">
+        <v>251</v>
+      </c>
+      <c r="O25" t="s">
+        <v>252</v>
+      </c>
+      <c r="P25" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>250</v>
+      </c>
+      <c r="R25" t="s">
+        <v>255</v>
+      </c>
+      <c r="S25" t="s">
+        <v>256</v>
+      </c>
+      <c r="T25" t="s">
         <v>203</v>
       </c>
-      <c r="L25" t="s">
+      <c r="U25" t="s">
+        <v>254</v>
+      </c>
+      <c r="V25" t="s">
         <v>250</v>
       </c>
-      <c r="M25" t="s">
-        <v>241</v>
-      </c>
-      <c r="N25" t="s">
-        <v>252</v>
-      </c>
-      <c r="O25" t="s">
-        <v>253</v>
-      </c>
-      <c r="P25" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>251</v>
-      </c>
-      <c r="R25" t="s">
-        <v>256</v>
-      </c>
-      <c r="S25" t="s">
+      <c r="W25" t="s">
         <v>257</v>
       </c>
-      <c r="T25" t="s">
-        <v>204</v>
-      </c>
-      <c r="U25" t="s">
-        <v>255</v>
-      </c>
-      <c r="V25" t="s">
-        <v>251</v>
-      </c>
-      <c r="W25" t="s">
-        <v>258</v>
-      </c>
       <c r="X25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA25" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1782,76 +1860,76 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>258</v>
+      </c>
+      <c r="G26" t="s">
         <v>259</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>260</v>
       </c>
-      <c r="H26" t="s">
-        <v>261</v>
-      </c>
       <c r="I26" t="s">
+        <v>263</v>
+      </c>
+      <c r="J26" t="s">
+        <v>275</v>
+      </c>
+      <c r="K26" t="s">
+        <v>270</v>
+      </c>
+      <c r="L26" t="s">
+        <v>264</v>
+      </c>
+      <c r="M26" t="s">
+        <v>269</v>
+      </c>
+      <c r="N26" t="s">
         <v>265</v>
       </c>
-      <c r="J26" t="s">
-        <v>277</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="O26" t="s">
+        <v>267</v>
+      </c>
+      <c r="P26" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>271</v>
+      </c>
+      <c r="R26" t="s">
+        <v>268</v>
+      </c>
+      <c r="S26" t="s">
         <v>272</v>
       </c>
-      <c r="L26" t="s">
-        <v>266</v>
-      </c>
-      <c r="M26" t="s">
-        <v>271</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="T26" t="s">
+        <v>273</v>
+      </c>
+      <c r="U26" t="s">
+        <v>274</v>
+      </c>
+      <c r="V26" t="s">
         <v>267</v>
       </c>
-      <c r="O26" t="s">
-        <v>269</v>
-      </c>
-      <c r="P26" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>273</v>
-      </c>
-      <c r="R26" t="s">
-        <v>270</v>
-      </c>
-      <c r="S26" t="s">
-        <v>274</v>
-      </c>
-      <c r="T26" t="s">
-        <v>275</v>
-      </c>
-      <c r="U26" t="s">
-        <v>276</v>
-      </c>
-      <c r="V26" t="s">
-        <v>269</v>
-      </c>
       <c r="W26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Y26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AA26" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1862,61 +1940,61 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" t="s">
+        <v>262</v>
+      </c>
+      <c r="H27" t="s">
+        <v>213</v>
+      </c>
+      <c r="I27" t="s">
+        <v>279</v>
+      </c>
+      <c r="J27" t="s">
+        <v>280</v>
+      </c>
+      <c r="K27" t="s">
+        <v>281</v>
+      </c>
+      <c r="L27" t="s">
         <v>206</v>
       </c>
-      <c r="G27" t="s">
-        <v>264</v>
-      </c>
-      <c r="H27" t="s">
-        <v>214</v>
-      </c>
-      <c r="I27" t="s">
-        <v>281</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="M27" t="s">
         <v>282</v>
       </c>
-      <c r="K27" t="s">
+      <c r="N27" t="s">
         <v>283</v>
       </c>
-      <c r="L27" t="s">
-        <v>207</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>284</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q27" t="s">
         <v>285</v>
       </c>
-      <c r="O27" t="s">
+      <c r="R27" t="s">
         <v>286</v>
       </c>
-      <c r="P27" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>287</v>
-      </c>
-      <c r="R27" t="s">
-        <v>288</v>
-      </c>
       <c r="S27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="T27" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AA27" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1927,55 +2005,55 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G28" t="s">
+        <v>296</v>
+      </c>
+      <c r="H28" t="s">
+        <v>297</v>
+      </c>
+      <c r="I28" t="s">
+        <v>299</v>
+      </c>
+      <c r="J28" t="s">
         <v>298</v>
       </c>
-      <c r="H28" t="s">
-        <v>299</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
+        <v>305</v>
+      </c>
+      <c r="L28" t="s">
+        <v>306</v>
+      </c>
+      <c r="M28" t="s">
+        <v>300</v>
+      </c>
+      <c r="N28" t="s">
         <v>301</v>
       </c>
-      <c r="J28" t="s">
-        <v>300</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="O28" t="s">
+        <v>215</v>
+      </c>
+      <c r="P28" t="s">
         <v>307</v>
       </c>
-      <c r="L28" t="s">
+      <c r="Q28" t="s">
         <v>308</v>
       </c>
-      <c r="M28" t="s">
+      <c r="R28" t="s">
         <v>302</v>
       </c>
-      <c r="N28" t="s">
-        <v>303</v>
-      </c>
-      <c r="O28" t="s">
-        <v>216</v>
-      </c>
-      <c r="P28" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>310</v>
-      </c>
-      <c r="R28" t="s">
-        <v>304</v>
-      </c>
       <c r="AA28" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1986,34 +2064,34 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G29" t="s">
+        <v>216</v>
+      </c>
+      <c r="H29" t="s">
         <v>217</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
+        <v>304</v>
+      </c>
+      <c r="J29" t="s">
+        <v>219</v>
+      </c>
+      <c r="K29" t="s">
         <v>218</v>
       </c>
-      <c r="I29" t="s">
-        <v>306</v>
-      </c>
-      <c r="J29" t="s">
-        <v>220</v>
-      </c>
-      <c r="K29" t="s">
-        <v>219</v>
-      </c>
       <c r="AA29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2024,43 +2102,43 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
       <c r="F30" t="s">
+        <v>314</v>
+      </c>
+      <c r="G30" t="s">
+        <v>324</v>
+      </c>
+      <c r="H30" t="s">
+        <v>220</v>
+      </c>
+      <c r="I30" t="s">
+        <v>315</v>
+      </c>
+      <c r="J30" t="s">
+        <v>221</v>
+      </c>
+      <c r="K30" t="s">
         <v>316</v>
       </c>
-      <c r="G30" t="s">
-        <v>326</v>
-      </c>
-      <c r="H30" t="s">
-        <v>221</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="L30" t="s">
+        <v>222</v>
+      </c>
+      <c r="M30" t="s">
+        <v>223</v>
+      </c>
+      <c r="N30" t="s">
         <v>317</v>
       </c>
-      <c r="J30" t="s">
-        <v>222</v>
-      </c>
-      <c r="K30" t="s">
-        <v>318</v>
-      </c>
-      <c r="L30" t="s">
-        <v>223</v>
-      </c>
-      <c r="M30" t="s">
-        <v>224</v>
-      </c>
-      <c r="N30" t="s">
-        <v>319</v>
-      </c>
       <c r="O30" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2071,34 +2149,34 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E31">
         <v>6</v>
       </c>
       <c r="F31" t="s">
+        <v>318</v>
+      </c>
+      <c r="G31" t="s">
+        <v>224</v>
+      </c>
+      <c r="H31" t="s">
+        <v>319</v>
+      </c>
+      <c r="I31" t="s">
+        <v>226</v>
+      </c>
+      <c r="J31" t="s">
         <v>320</v>
       </c>
-      <c r="G31" t="s">
-        <v>225</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="K31" t="s">
         <v>321</v>
       </c>
-      <c r="I31" t="s">
-        <v>227</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="L31" t="s">
         <v>322</v>
       </c>
-      <c r="K31" t="s">
-        <v>323</v>
-      </c>
-      <c r="L31" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2109,13 +2187,76 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E32">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>329</v>
+      </c>
+      <c r="G32" t="s">
+        <v>235</v>
+      </c>
+      <c r="H32" t="s">
+        <v>228</v>
+      </c>
+      <c r="I32" t="s">
+        <v>229</v>
+      </c>
+      <c r="J32" t="s">
+        <v>330</v>
+      </c>
+      <c r="K32" t="s">
+        <v>331</v>
+      </c>
+      <c r="L32" t="s">
+        <v>332</v>
+      </c>
+      <c r="M32" t="s">
+        <v>333</v>
+      </c>
+      <c r="N32" t="s">
+        <v>334</v>
+      </c>
+      <c r="O32" t="s">
+        <v>335</v>
+      </c>
+      <c r="P32" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>337</v>
+      </c>
+      <c r="R32" t="s">
+        <v>338</v>
+      </c>
+      <c r="S32" t="s">
+        <v>339</v>
+      </c>
+      <c r="T32" t="s">
+        <v>340</v>
+      </c>
+      <c r="U32" t="s">
+        <v>341</v>
+      </c>
+      <c r="V32" t="s">
+        <v>342</v>
+      </c>
+      <c r="W32" t="s">
+        <v>343</v>
+      </c>
+      <c r="X32" t="s">
+        <v>344</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2126,13 +2267,46 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>347</v>
+      </c>
+      <c r="G33" t="s">
+        <v>348</v>
+      </c>
+      <c r="H33" t="s">
+        <v>349</v>
+      </c>
+      <c r="I33" t="s">
+        <v>350</v>
+      </c>
+      <c r="J33" t="s">
+        <v>351</v>
+      </c>
+      <c r="K33" t="s">
+        <v>352</v>
+      </c>
+      <c r="L33" t="s">
+        <v>353</v>
+      </c>
+      <c r="M33" t="s">
+        <v>354</v>
+      </c>
+      <c r="N33" t="s">
+        <v>355</v>
+      </c>
+      <c r="O33" t="s">
+        <v>329</v>
+      </c>
+      <c r="P33" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2143,13 +2317,13 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2160,10 +2334,10 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2174,38 +2348,38 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2216,10 +2390,10 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2230,10 +2404,10 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2244,10 +2418,10 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2258,10 +2432,10 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2272,10 +2446,10 @@
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2286,10 +2460,10 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2300,10 +2474,10 @@
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2314,10 +2488,10 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2328,10 +2502,10 @@
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2342,10 +2516,10 @@
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2356,10 +2530,10 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2370,38 +2544,38 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C52">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2412,10 +2586,10 @@
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2426,10 +2600,10 @@
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2440,10 +2614,10 @@
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2454,10 +2628,10 @@
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2468,38 +2642,38 @@
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2510,10 +2684,10 @@
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2521,7 +2695,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2529,7 +2703,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2537,15 +2711,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2553,7 +2727,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2561,7 +2735,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2569,7 +2743,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2577,7 +2751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2585,7 +2759,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2593,7 +2767,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2601,7 +2775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2609,7 +2783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2617,7 +2791,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2625,7 +2799,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2633,7 +2807,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2641,7 +2815,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2649,7 +2823,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2657,7 +2831,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2665,7 +2839,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2673,7 +2847,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2681,7 +2855,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2689,307 +2863,307 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
         <v>146</v>
       </c>
-      <c r="C85" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Eggs and some bug fixes!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3EAD8-FAFE-4710-AFDB-383F7B75FDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34B1CD0-1135-4D9E-B5F4-B73AC929E420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="358">
   <si>
     <t>Current</t>
   </si>
@@ -1107,6 +1107,9 @@
   </si>
   <si>
     <t>Champion</t>
+  </si>
+  <si>
+    <t>Res A Gift</t>
   </si>
 </sst>
 </file>
@@ -1486,17 +1489,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AA142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.6640625" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1692,7 +1695,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1772,7 +1775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1925,11 +1928,14 @@
       <c r="Y26" t="s">
         <v>327</v>
       </c>
+      <c r="Z26" t="s">
+        <v>357</v>
+      </c>
       <c r="AA26" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2138,7 +2144,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2176,7 +2182,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2256,7 +2262,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2337,7 +2343,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2379,7 +2385,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2491,7 +2497,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2533,7 +2539,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2575,7 +2581,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2659,7 +2665,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2687,7 +2693,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2711,7 +2717,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2727,7 +2733,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2735,7 +2741,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2767,7 +2773,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2783,7 +2789,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2791,7 +2797,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2799,7 +2805,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2815,7 +2821,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2823,7 +2829,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2855,7 +2861,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2863,17 +2869,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -2881,287 +2887,287 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
Casino story sync work!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34B1CD0-1135-4D9E-B5F4-B73AC929E420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CE7A4C-E7A9-45E3-A9A2-69AABA0F4469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="359">
   <si>
     <t>Current</t>
   </si>
@@ -1110,6 +1110,9 @@
   </si>
   <si>
     <t>Res A Gift</t>
+  </si>
+  <si>
+    <t>Guy Eddie</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1493,7 @@
   <dimension ref="A1:AA142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,6 +1851,9 @@
       <c r="X25" t="s">
         <v>234</v>
       </c>
+      <c r="Y25" t="s">
+        <v>358</v>
+      </c>
       <c r="AA25" t="s">
         <v>309</v>
       </c>

</xml_diff>

<commit_message>
Implemented all moves except Trick Tackle and more TM work!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C6CE65-824C-4BE3-88B7-3A06C1C764A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666C85C3-0E03-4B3F-BF68-3CFCC17FAFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="373">
   <si>
     <t>Current</t>
   </si>
@@ -1119,6 +1119,42 @@
   </si>
   <si>
     <t>All E Forms</t>
+  </si>
+  <si>
+    <t>Shake 1</t>
+  </si>
+  <si>
+    <t>Shake 2</t>
+  </si>
+  <si>
+    <t>Shake 3</t>
+  </si>
+  <si>
+    <t>Shake 4</t>
+  </si>
+  <si>
+    <t>Shake 5</t>
+  </si>
+  <si>
+    <t>Shake 6</t>
+  </si>
+  <si>
+    <t>Shake 7</t>
+  </si>
+  <si>
+    <t>Shake 8</t>
+  </si>
+  <si>
+    <t>Shake 9</t>
+  </si>
+  <si>
+    <t>Shake 10</t>
+  </si>
+  <si>
+    <t>Shake 11</t>
+  </si>
+  <si>
+    <t>Shake 12</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1535,7 @@
   <dimension ref="A1:AB142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+      <selection activeCell="Y31" sqref="Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,6 +2241,42 @@
       <c r="L31" t="s">
         <v>322</v>
       </c>
+      <c r="M31" t="s">
+        <v>361</v>
+      </c>
+      <c r="N31" t="s">
+        <v>362</v>
+      </c>
+      <c r="O31" t="s">
+        <v>363</v>
+      </c>
+      <c r="P31" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>365</v>
+      </c>
+      <c r="R31" t="s">
+        <v>366</v>
+      </c>
+      <c r="S31" t="s">
+        <v>367</v>
+      </c>
+      <c r="T31" t="s">
+        <v>368</v>
+      </c>
+      <c r="U31" t="s">
+        <v>369</v>
+      </c>
+      <c r="V31" t="s">
+        <v>370</v>
+      </c>
+      <c r="W31" t="s">
+        <v>371</v>
+      </c>
+      <c r="X31" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
Vegas work: new items in overworld and bug fixes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666C85C3-0E03-4B3F-BF68-3CFCC17FAFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDE2599-F8FB-4C51-B3DF-535D14C8220C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="376">
   <si>
     <t>Current</t>
   </si>
@@ -1155,6 +1155,15 @@
   </si>
   <si>
     <t>Shake 12</t>
+  </si>
+  <si>
+    <t>All S Forms</t>
+  </si>
+  <si>
+    <t>1+ S Forms</t>
+  </si>
+  <si>
+    <t>Shell Bell</t>
   </si>
 </sst>
 </file>
@@ -1534,17 +1543,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="Y31" sqref="Y31"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.7109375" customWidth="1"/>
+    <col min="2" max="2" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1564,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1566,7 +1575,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1602,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1620,7 +1629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1660,7 +1669,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1717,7 +1726,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1917,8 +1926,17 @@
       <c r="Y25" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z25" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>373</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2004,7 +2022,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2066,7 +2084,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2122,7 +2140,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2157,7 +2175,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2204,7 +2222,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2358,7 +2376,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2408,7 +2426,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2425,7 +2443,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2439,7 +2457,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2453,7 +2471,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2467,7 +2485,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2481,7 +2499,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2495,7 +2513,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2509,7 +2527,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2523,7 +2541,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2537,7 +2555,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2551,7 +2569,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2565,7 +2583,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2579,7 +2597,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2593,7 +2611,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2607,7 +2625,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2621,7 +2639,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2635,7 +2653,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2649,7 +2667,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2663,7 +2681,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2677,7 +2695,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2691,7 +2709,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2705,7 +2723,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2719,7 +2737,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2733,7 +2751,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2747,7 +2765,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2761,7 +2779,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2775,7 +2793,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2789,7 +2807,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2797,7 +2815,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2805,7 +2823,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2813,7 +2831,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2821,7 +2839,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2829,7 +2847,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2837,7 +2855,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2845,7 +2863,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2853,7 +2871,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2861,7 +2879,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2869,7 +2887,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2877,7 +2895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2885,7 +2903,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2893,7 +2911,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2901,7 +2919,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2909,7 +2927,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2917,7 +2935,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2925,7 +2943,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2933,7 +2951,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2941,7 +2959,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2949,7 +2967,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2957,7 +2975,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2965,17 +2983,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -2983,287 +3001,287 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
8th gym split script work, bug fixes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDE2599-F8FB-4C51-B3DF-535D14C8220C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2889CCBC-9A90-425A-B41A-983B79D9E37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="377">
   <si>
     <t>Current</t>
   </si>
@@ -1164,6 +1164,9 @@
   </si>
   <si>
     <t>Shell Bell</t>
+  </si>
+  <si>
+    <t>Merlin coming</t>
   </si>
 </sst>
 </file>
@@ -1543,17 +1546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.6640625" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2175,7 +2178,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2316,67 +2319,70 @@
         <v>329</v>
       </c>
       <c r="G32" t="s">
+        <v>376</v>
+      </c>
+      <c r="H32" t="s">
         <v>235</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>228</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>229</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>330</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>331</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>332</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>333</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>334</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>335</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>336</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>337</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>338</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>339</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>340</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>341</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>342</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>343</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>344</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>345</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AA32" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2426,7 +2432,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2457,7 +2463,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2513,7 +2519,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2569,7 +2575,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2611,7 +2617,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2653,7 +2659,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2681,7 +2687,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2779,7 +2785,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2815,7 +2821,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2823,7 +2829,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2855,7 +2861,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2871,7 +2877,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2879,7 +2885,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2887,7 +2893,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2895,7 +2901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2911,7 +2917,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2943,7 +2949,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2951,7 +2957,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2959,7 +2965,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2967,7 +2973,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2975,7 +2981,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2983,17 +2989,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -3001,287 +3007,287 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
8th gym split work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2889CCBC-9A90-425A-B41A-983B79D9E37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7596CA84-E947-4E2E-89A3-A69C25D1FDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -1546,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Magic spell task done and extra text for Arthra and Merlin after scene
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7596CA84-E947-4E2E-89A3-A69C25D1FDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE26574-956C-404C-8B54-E497C4FE2659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1546,17 +1546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="B92" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.7109375" customWidth="1"/>
+    <col min="2" max="2" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2989,17 +2989,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -3007,287 +3007,287 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
New sprite, and 8th gym split work (ghostly woods heart done!)
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE26574-956C-404C-8B54-E497C4FE2659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C44D7E2-5DE6-45BD-9745-A6A4A6F7A147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,9 +557,6 @@
     <t>Dragowrath appears and gets mad that you took his kid, big fight against a +6 Dragowrath and your legendary, you are forced to lose</t>
   </si>
   <si>
-    <t>Dragowrath monogues about how it's not enough, your belief was wrong it's not enough, Arthia suffered a similar fate her belief was wrong too</t>
-  </si>
-  <si>
     <t>Merlin gets possessed once you white out, he's too weak to defend himself, his last spell was teleporting you guys to safety</t>
   </si>
   <si>
@@ -584,18 +581,12 @@
     <t>Awake the legendary with the help of Merlin and the meteorite energy rock thing, fight and force capture</t>
   </si>
   <si>
-    <t>Arthia realizes that to be worthy she can't do it alone, she needs your help too. You guys realize that the only space station is in Iron Town and that Dragowrath is in space</t>
-  </si>
-  <si>
     <t>On Route 39 you guys reach the shack, Ryder is in there alone trying to figure out what the hell is going on, you guys explain it to him and that you need to go to space</t>
   </si>
   <si>
     <t>You 3 make it to Iron Town, Ryder starts being possessed, Alakazam comes out and takes control of his body, helps you guys fly the spaceship</t>
   </si>
   <si>
-    <t>You guys manage to make it to space, see Dragowrath there, somehow you and Arthia teamwork beat it, Dragowrath frees Earth but you guys are stuck here</t>
-  </si>
-  <si>
     <t>You explore to find Nova's gym, she was Dragowrath's sidekick but her boss is defeated, she says she can take you back to Earth but you have to prove you're worthy</t>
   </si>
   <si>
@@ -1167,6 +1158,15 @@
   </si>
   <si>
     <t>Merlin coming</t>
+  </si>
+  <si>
+    <t>Dragowrath monogues about how it's not enough, your belief was wrong it's not enough, Arthra suffered a similar fate her belief was wrong too</t>
+  </si>
+  <si>
+    <t>Arthra realizes that to be worthy she can't do it alone, she needs your help too. You guys realize that the only space station is in Iron Town and that Dragowrath is in space</t>
+  </si>
+  <si>
+    <t>You guys manage to make it to space, see Dragowrath there, somehow you and Arthra teamwork beat it, Dragowrath frees Earth but you guys are stuck here</t>
   </si>
 </sst>
 </file>
@@ -1546,17 +1546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B92" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.6640625" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1564,10 +1564,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1613,10 +1613,10 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1696,18 +1696,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="Z17" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1715,10 +1715,10 @@
         <v>91</v>
       </c>
       <c r="Z18" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1726,10 +1726,10 @@
         <v>92</v>
       </c>
       <c r="Z19" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1737,29 +1737,29 @@
         <v>93</v>
       </c>
       <c r="Z20" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="Z21" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1778,10 +1778,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E24" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1853,93 +1853,93 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H25" t="s">
+        <v>242</v>
+      </c>
+      <c r="I25" t="s">
+        <v>236</v>
+      </c>
+      <c r="J25" t="s">
         <v>245</v>
       </c>
-      <c r="I25" t="s">
-        <v>239</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
+        <v>199</v>
+      </c>
+      <c r="L25" t="s">
+        <v>246</v>
+      </c>
+      <c r="M25" t="s">
+        <v>237</v>
+      </c>
+      <c r="N25" t="s">
         <v>248</v>
       </c>
-      <c r="K25" t="s">
-        <v>202</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="O25" t="s">
         <v>249</v>
       </c>
-      <c r="M25" t="s">
-        <v>240</v>
-      </c>
-      <c r="N25" t="s">
+      <c r="P25" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>247</v>
+      </c>
+      <c r="R25" t="s">
+        <v>252</v>
+      </c>
+      <c r="S25" t="s">
+        <v>253</v>
+      </c>
+      <c r="T25" t="s">
+        <v>200</v>
+      </c>
+      <c r="U25" t="s">
         <v>251</v>
       </c>
-      <c r="O25" t="s">
-        <v>252</v>
-      </c>
-      <c r="P25" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>250</v>
-      </c>
-      <c r="R25" t="s">
-        <v>255</v>
-      </c>
-      <c r="S25" t="s">
-        <v>256</v>
-      </c>
-      <c r="T25" t="s">
-        <v>203</v>
-      </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
+        <v>247</v>
+      </c>
+      <c r="W25" t="s">
         <v>254</v>
       </c>
-      <c r="V25" t="s">
-        <v>250</v>
-      </c>
-      <c r="W25" t="s">
-        <v>257</v>
-      </c>
       <c r="X25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Y25" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Z25" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="AA25" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AB25" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1950,82 +1950,82 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G26" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H26" t="s">
+        <v>257</v>
+      </c>
+      <c r="I26" t="s">
         <v>260</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
+        <v>272</v>
+      </c>
+      <c r="K26" t="s">
+        <v>267</v>
+      </c>
+      <c r="L26" t="s">
+        <v>261</v>
+      </c>
+      <c r="M26" t="s">
+        <v>266</v>
+      </c>
+      <c r="N26" t="s">
+        <v>262</v>
+      </c>
+      <c r="O26" t="s">
+        <v>264</v>
+      </c>
+      <c r="P26" t="s">
         <v>263</v>
       </c>
-      <c r="J26" t="s">
+      <c r="Q26" t="s">
+        <v>268</v>
+      </c>
+      <c r="R26" t="s">
+        <v>265</v>
+      </c>
+      <c r="S26" t="s">
+        <v>269</v>
+      </c>
+      <c r="T26" t="s">
+        <v>270</v>
+      </c>
+      <c r="U26" t="s">
+        <v>271</v>
+      </c>
+      <c r="V26" t="s">
+        <v>264</v>
+      </c>
+      <c r="W26" t="s">
+        <v>228</v>
+      </c>
+      <c r="X26" t="s">
         <v>275</v>
       </c>
-      <c r="K26" t="s">
-        <v>270</v>
-      </c>
-      <c r="L26" t="s">
-        <v>264</v>
-      </c>
-      <c r="M26" t="s">
-        <v>269</v>
-      </c>
-      <c r="N26" t="s">
-        <v>265</v>
-      </c>
-      <c r="O26" t="s">
-        <v>267</v>
-      </c>
-      <c r="P26" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>271</v>
-      </c>
-      <c r="R26" t="s">
-        <v>268</v>
-      </c>
-      <c r="S26" t="s">
-        <v>272</v>
-      </c>
-      <c r="T26" t="s">
-        <v>273</v>
-      </c>
-      <c r="U26" t="s">
-        <v>274</v>
-      </c>
-      <c r="V26" t="s">
-        <v>267</v>
-      </c>
-      <c r="W26" t="s">
-        <v>231</v>
-      </c>
-      <c r="X26" t="s">
-        <v>278</v>
-      </c>
       <c r="Y26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Z26" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>356</v>
+      </c>
+      <c r="AB26" t="s">
         <v>357</v>
       </c>
-      <c r="AA26" t="s">
-        <v>359</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2036,58 +2036,58 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G27" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H27" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I27" t="s">
+        <v>276</v>
+      </c>
+      <c r="J27" t="s">
+        <v>277</v>
+      </c>
+      <c r="K27" t="s">
+        <v>278</v>
+      </c>
+      <c r="L27" t="s">
+        <v>203</v>
+      </c>
+      <c r="M27" t="s">
         <v>279</v>
       </c>
-      <c r="J27" t="s">
+      <c r="N27" t="s">
         <v>280</v>
       </c>
-      <c r="K27" t="s">
+      <c r="O27" t="s">
         <v>281</v>
       </c>
-      <c r="L27" t="s">
-        <v>206</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="P27" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q27" t="s">
         <v>282</v>
       </c>
-      <c r="N27" t="s">
+      <c r="R27" t="s">
         <v>283</v>
       </c>
-      <c r="O27" t="s">
-        <v>284</v>
-      </c>
-      <c r="P27" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>285</v>
-      </c>
-      <c r="R27" t="s">
-        <v>286</v>
-      </c>
       <c r="S27" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="T27" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2098,52 +2098,52 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28" t="s">
+        <v>290</v>
+      </c>
+      <c r="G28" t="s">
         <v>293</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
+        <v>294</v>
+      </c>
+      <c r="I28" t="s">
         <v>296</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
+        <v>295</v>
+      </c>
+      <c r="K28" t="s">
+        <v>302</v>
+      </c>
+      <c r="L28" t="s">
+        <v>303</v>
+      </c>
+      <c r="M28" t="s">
         <v>297</v>
       </c>
-      <c r="I28" t="s">
+      <c r="N28" t="s">
+        <v>298</v>
+      </c>
+      <c r="O28" t="s">
+        <v>212</v>
+      </c>
+      <c r="P28" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>305</v>
+      </c>
+      <c r="R28" t="s">
         <v>299</v>
       </c>
-      <c r="J28" t="s">
-        <v>298</v>
-      </c>
-      <c r="K28" t="s">
-        <v>305</v>
-      </c>
-      <c r="L28" t="s">
-        <v>306</v>
-      </c>
-      <c r="M28" t="s">
-        <v>300</v>
-      </c>
-      <c r="N28" t="s">
-        <v>301</v>
-      </c>
-      <c r="O28" t="s">
-        <v>215</v>
-      </c>
-      <c r="P28" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>308</v>
-      </c>
-      <c r="R28" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2154,31 +2154,31 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G29" t="s">
+        <v>213</v>
+      </c>
+      <c r="H29" t="s">
+        <v>214</v>
+      </c>
+      <c r="I29" t="s">
+        <v>301</v>
+      </c>
+      <c r="J29" t="s">
         <v>216</v>
       </c>
-      <c r="H29" t="s">
-        <v>217</v>
-      </c>
-      <c r="I29" t="s">
-        <v>304</v>
-      </c>
-      <c r="J29" t="s">
-        <v>219</v>
-      </c>
       <c r="K29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2189,43 +2189,43 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
       <c r="F30" t="s">
+        <v>311</v>
+      </c>
+      <c r="G30" t="s">
+        <v>321</v>
+      </c>
+      <c r="H30" t="s">
+        <v>217</v>
+      </c>
+      <c r="I30" t="s">
+        <v>312</v>
+      </c>
+      <c r="J30" t="s">
+        <v>218</v>
+      </c>
+      <c r="K30" t="s">
+        <v>313</v>
+      </c>
+      <c r="L30" t="s">
+        <v>219</v>
+      </c>
+      <c r="M30" t="s">
+        <v>220</v>
+      </c>
+      <c r="N30" t="s">
         <v>314</v>
       </c>
-      <c r="G30" t="s">
-        <v>324</v>
-      </c>
-      <c r="H30" t="s">
-        <v>220</v>
-      </c>
-      <c r="I30" t="s">
-        <v>315</v>
-      </c>
-      <c r="J30" t="s">
-        <v>221</v>
-      </c>
-      <c r="K30" t="s">
-        <v>316</v>
-      </c>
-      <c r="L30" t="s">
-        <v>222</v>
-      </c>
-      <c r="M30" t="s">
-        <v>223</v>
-      </c>
-      <c r="N30" t="s">
-        <v>317</v>
-      </c>
       <c r="O30" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2236,70 +2236,70 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E31">
         <v>6</v>
       </c>
       <c r="F31" t="s">
+        <v>315</v>
+      </c>
+      <c r="G31" t="s">
+        <v>221</v>
+      </c>
+      <c r="H31" t="s">
+        <v>316</v>
+      </c>
+      <c r="I31" t="s">
+        <v>223</v>
+      </c>
+      <c r="J31" t="s">
+        <v>317</v>
+      </c>
+      <c r="K31" t="s">
         <v>318</v>
       </c>
-      <c r="G31" t="s">
-        <v>224</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="L31" t="s">
         <v>319</v>
       </c>
-      <c r="I31" t="s">
-        <v>226</v>
-      </c>
-      <c r="J31" t="s">
-        <v>320</v>
-      </c>
-      <c r="K31" t="s">
-        <v>321</v>
-      </c>
-      <c r="L31" t="s">
-        <v>322</v>
-      </c>
       <c r="M31" t="s">
+        <v>358</v>
+      </c>
+      <c r="N31" t="s">
+        <v>359</v>
+      </c>
+      <c r="O31" t="s">
+        <v>360</v>
+      </c>
+      <c r="P31" t="s">
         <v>361</v>
       </c>
-      <c r="N31" t="s">
+      <c r="Q31" t="s">
         <v>362</v>
       </c>
-      <c r="O31" t="s">
+      <c r="R31" t="s">
         <v>363</v>
       </c>
-      <c r="P31" t="s">
+      <c r="S31" t="s">
         <v>364</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="T31" t="s">
         <v>365</v>
       </c>
-      <c r="R31" t="s">
+      <c r="U31" t="s">
         <v>366</v>
       </c>
-      <c r="S31" t="s">
+      <c r="V31" t="s">
         <v>367</v>
       </c>
-      <c r="T31" t="s">
+      <c r="W31" t="s">
         <v>368</v>
       </c>
-      <c r="U31" t="s">
+      <c r="X31" t="s">
         <v>369</v>
       </c>
-      <c r="V31" t="s">
-        <v>370</v>
-      </c>
-      <c r="W31" t="s">
-        <v>371</v>
-      </c>
-      <c r="X31" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2310,79 +2310,79 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E32">
         <v>7</v>
       </c>
       <c r="F32" t="s">
+        <v>326</v>
+      </c>
+      <c r="G32" t="s">
+        <v>373</v>
+      </c>
+      <c r="H32" t="s">
+        <v>232</v>
+      </c>
+      <c r="I32" t="s">
+        <v>225</v>
+      </c>
+      <c r="J32" t="s">
+        <v>226</v>
+      </c>
+      <c r="K32" t="s">
+        <v>327</v>
+      </c>
+      <c r="L32" t="s">
+        <v>328</v>
+      </c>
+      <c r="M32" t="s">
         <v>329</v>
       </c>
-      <c r="G32" t="s">
-        <v>376</v>
-      </c>
-      <c r="H32" t="s">
-        <v>235</v>
-      </c>
-      <c r="I32" t="s">
-        <v>228</v>
-      </c>
-      <c r="J32" t="s">
-        <v>229</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="N32" t="s">
         <v>330</v>
       </c>
-      <c r="L32" t="s">
+      <c r="O32" t="s">
+        <v>332</v>
+      </c>
+      <c r="P32" t="s">
         <v>331</v>
       </c>
-      <c r="M32" t="s">
-        <v>332</v>
-      </c>
-      <c r="N32" t="s">
+      <c r="Q32" t="s">
         <v>333</v>
       </c>
-      <c r="O32" t="s">
+      <c r="R32" t="s">
         <v>334</v>
       </c>
-      <c r="P32" t="s">
+      <c r="S32" t="s">
         <v>335</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="T32" t="s">
         <v>336</v>
       </c>
-      <c r="R32" t="s">
+      <c r="U32" t="s">
         <v>337</v>
       </c>
-      <c r="S32" t="s">
+      <c r="V32" t="s">
         <v>338</v>
       </c>
-      <c r="T32" t="s">
+      <c r="W32" t="s">
         <v>339</v>
       </c>
-      <c r="U32" t="s">
+      <c r="X32" t="s">
         <v>340</v>
       </c>
-      <c r="V32" t="s">
+      <c r="Y32" t="s">
         <v>341</v>
       </c>
-      <c r="W32" t="s">
+      <c r="Z32" t="s">
         <v>342</v>
       </c>
-      <c r="X32" t="s">
+      <c r="AA32" t="s">
         <v>343</v>
       </c>
-      <c r="Y32" t="s">
-        <v>344</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>345</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2393,46 +2393,46 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
       </c>
       <c r="F33" t="s">
+        <v>344</v>
+      </c>
+      <c r="G33" t="s">
+        <v>345</v>
+      </c>
+      <c r="H33" t="s">
+        <v>346</v>
+      </c>
+      <c r="I33" t="s">
         <v>347</v>
       </c>
-      <c r="G33" t="s">
+      <c r="J33" t="s">
         <v>348</v>
       </c>
-      <c r="H33" t="s">
+      <c r="K33" t="s">
         <v>349</v>
       </c>
-      <c r="I33" t="s">
+      <c r="L33" t="s">
         <v>350</v>
       </c>
-      <c r="J33" t="s">
+      <c r="M33" t="s">
         <v>351</v>
       </c>
-      <c r="K33" t="s">
+      <c r="N33" t="s">
         <v>352</v>
       </c>
-      <c r="L33" t="s">
+      <c r="O33" t="s">
+        <v>326</v>
+      </c>
+      <c r="P33" t="s">
         <v>353</v>
       </c>
-      <c r="M33" t="s">
-        <v>354</v>
-      </c>
-      <c r="N33" t="s">
-        <v>355</v>
-      </c>
-      <c r="O33" t="s">
-        <v>329</v>
-      </c>
-      <c r="P33" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2443,13 +2443,13 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2460,10 +2460,10 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2474,38 +2474,38 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C37">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2516,10 +2516,10 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2530,10 +2530,10 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2544,10 +2544,10 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2558,10 +2558,10 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2572,10 +2572,10 @@
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2586,10 +2586,10 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2600,10 +2600,10 @@
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2614,10 +2614,10 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2628,10 +2628,10 @@
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2642,10 +2642,10 @@
         <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2656,10 +2656,10 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2670,38 +2670,38 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C51">
         <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C52">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2712,10 +2712,10 @@
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2726,10 +2726,10 @@
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2740,10 +2740,10 @@
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2754,10 +2754,10 @@
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2768,38 +2768,38 @@
         <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C58">
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C59">
         <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2810,10 +2810,10 @@
         <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2837,15 +2837,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2989,17 +2989,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -3007,289 +3007,289 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B113" t="s">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B114" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B118" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B121" t="s">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B122" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B129" t="s">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B130" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B131" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B132" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B135" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B136" t="s">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B137" t="s">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B138" t="s">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B139" t="s">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B140" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B141" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B142" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AT Path/Abandoned Tower exterior work, bug fixes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C44D7E2-5DE6-45BD-9745-A6A4A6F7A147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2489B041-956B-48DA-A90D-3CD2F3E75823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="379">
   <si>
     <t>Current</t>
   </si>
@@ -1167,6 +1167,12 @@
   </si>
   <si>
     <t>You guys manage to make it to space, see Dragowrath there, somehow you and Arthra teamwork beat it, Dragowrath frees Earth but you guys are stuck here</t>
+  </si>
+  <si>
+    <t>Merlin Guide</t>
+  </si>
+  <si>
+    <t>Guard</t>
   </si>
 </sst>
 </file>
@@ -1544,16 +1550,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:AB142"/>
+  <dimension ref="A1:AC142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="105.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1696,7 +1703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1718,7 +1725,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1729,7 +1736,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1740,7 +1747,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1751,7 +1758,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1766,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1774,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1852,8 +1859,11 @@
       <c r="AB24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1939,7 +1949,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2087,7 +2097,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2143,7 +2153,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2178,7 +2188,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2225,7 +2235,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2299,7 +2309,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2349,36 +2359,42 @@
         <v>331</v>
       </c>
       <c r="Q32" t="s">
+        <v>377</v>
+      </c>
+      <c r="R32" t="s">
+        <v>378</v>
+      </c>
+      <c r="S32" t="s">
         <v>333</v>
       </c>
-      <c r="R32" t="s">
+      <c r="T32" t="s">
         <v>334</v>
       </c>
-      <c r="S32" t="s">
+      <c r="U32" t="s">
         <v>335</v>
       </c>
-      <c r="T32" t="s">
+      <c r="V32" t="s">
         <v>336</v>
       </c>
-      <c r="U32" t="s">
+      <c r="W32" t="s">
         <v>337</v>
       </c>
-      <c r="V32" t="s">
+      <c r="X32" t="s">
         <v>338</v>
       </c>
-      <c r="W32" t="s">
+      <c r="Y32" t="s">
         <v>339</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Z32" t="s">
         <v>340</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="AA32" t="s">
         <v>341</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AB32" t="s">
         <v>342</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AC32" t="s">
         <v>343</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fixes, new doc! and tm locations added to ItemInfo
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2489B041-956B-48DA-A90D-3CD2F3E75823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C9A098-EC5D-4767-9FFF-A1131F819179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1552,14 +1552,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AC142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.7109375" customWidth="1"/>
+    <col min="2" max="2" width="153.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
DID ALL OF ABANDONED TOWER + CUTSCENES!!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C9A098-EC5D-4767-9FFF-A1131F819179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AA9EE7-3B04-4769-A37B-3AB7BB8DB8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1552,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AC142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121:B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished Deep Chasm and got logic dragon overworld sprites!!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D9361-B98F-4C54-A47F-214244C6885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D90007F-AEFB-418A-84D4-FB0816E3A621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="380">
   <si>
     <t>Current</t>
   </si>
@@ -1173,6 +1173,9 @@
   </si>
   <si>
     <t>Guard</t>
+  </si>
+  <si>
+    <t>Arthra after</t>
   </si>
 </sst>
 </file>
@@ -1550,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:AC142"/>
+  <dimension ref="A1:AD142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="AE26" sqref="AE26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1706,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1766,7 +1769,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1862,8 +1865,11 @@
       <c r="AC24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2097,7 +2103,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2235,7 +2241,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2309,7 +2315,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2377,24 +2383,27 @@
         <v>336</v>
       </c>
       <c r="W32" t="s">
+        <v>379</v>
+      </c>
+      <c r="X32" t="s">
         <v>337</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>338</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>339</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AA32" t="s">
         <v>340</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>341</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AC32" t="s">
         <v>342</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AD32" t="s">
         <v>343</v>
       </c>
     </row>

</xml_diff>

<commit_message>
8th gym work on everything up to getting to space!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D90007F-AEFB-418A-84D4-FB0816E3A621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52231666-B21D-4DE9-A55D-6C3698C340E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AD142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="AE26" sqref="AE26"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Outer space Dragowrath boss fight complete!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52231666-B21D-4DE9-A55D-6C3698C340E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0391E1-5066-4588-BBC2-6E1A5BE1AB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -1058,9 +1058,6 @@
     <t>Get in Ship</t>
   </si>
   <si>
-    <t>Arthra Space</t>
-  </si>
-  <si>
     <t>Dragowrath</t>
   </si>
   <si>
@@ -1176,6 +1173,9 @@
   </si>
   <si>
     <t>Arthra after</t>
+  </si>
+  <si>
+    <t>Split for Nova</t>
   </si>
 </sst>
 </file>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AD142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="AD33" sqref="AD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,16 +1943,16 @@
         <v>231</v>
       </c>
       <c r="Y25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Z25" t="s">
+        <v>370</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB25" t="s">
         <v>371</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>370</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -2032,13 +2032,13 @@
         <v>324</v>
       </c>
       <c r="Z26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AA26" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB26" t="s">
         <v>356</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -2279,40 +2279,40 @@
         <v>319</v>
       </c>
       <c r="M31" t="s">
+        <v>357</v>
+      </c>
+      <c r="N31" t="s">
         <v>358</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>359</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>360</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>361</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>362</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>363</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>364</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>365</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>366</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>367</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>368</v>
-      </c>
-      <c r="X31" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -2335,7 +2335,7 @@
         <v>326</v>
       </c>
       <c r="G32" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H32" t="s">
         <v>232</v>
@@ -2365,10 +2365,10 @@
         <v>331</v>
       </c>
       <c r="Q32" t="s">
+        <v>376</v>
+      </c>
+      <c r="R32" t="s">
         <v>377</v>
-      </c>
-      <c r="R32" t="s">
-        <v>378</v>
       </c>
       <c r="S32" t="s">
         <v>333</v>
@@ -2383,7 +2383,7 @@
         <v>336</v>
       </c>
       <c r="W32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="X32" t="s">
         <v>337</v>
@@ -2398,13 +2398,13 @@
         <v>340</v>
       </c>
       <c r="AB32" t="s">
+        <v>379</v>
+      </c>
+      <c r="AC32" t="s">
         <v>341</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AD32" t="s">
         <v>342</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2424,37 +2424,37 @@
         <v>8</v>
       </c>
       <c r="F33" t="s">
+        <v>343</v>
+      </c>
+      <c r="G33" t="s">
         <v>344</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>345</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>346</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>347</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>348</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>349</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>350</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>351</v>
-      </c>
-      <c r="N33" t="s">
-        <v>352</v>
       </c>
       <c r="O33" t="s">
         <v>326</v>
       </c>
       <c r="P33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
@@ -3219,7 +3219,7 @@
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
@@ -3234,7 +3234,7 @@
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated NPC/Gym Leader sprites (from DeviantArt) and gym 8/E4 split work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0391E1-5066-4588-BBC2-6E1A5BE1AB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBA4843-588E-411B-A181-63F3475D0201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="392">
   <si>
     <t>Current</t>
   </si>
@@ -1176,6 +1176,42 @@
   </si>
   <si>
     <t>Split for Nova</t>
+  </si>
+  <si>
+    <t>In order to summon Dragowrath to catch, the player must get Merlin's staff (from the final room of the gauntlet they chose and captured one of the dragon's at)</t>
+  </si>
+  <si>
+    <t>The staff appears after the player gets back from outer space and saves Earth</t>
+  </si>
+  <si>
+    <t>Once they beat Arthra in the Elite Four, she has dialogue that says that she'll set her dragon free (for the player to catch), it goes back to its original resting place (other gauntlet)</t>
+  </si>
+  <si>
+    <t>Then the player can now go into that gauntlet too, and catch the other legendary Dragon</t>
+  </si>
+  <si>
+    <t>Once the champion is beat, Nova goes back to her house in outer space (in the cave system next to the gym)</t>
+  </si>
+  <si>
+    <t>Talking to Nova will ask the player if they're trying to track down Dragowrath, and she'll say he will only appear once the player has both Dragons</t>
+  </si>
+  <si>
+    <t>If have both Dragons but hasn't gotten Merlin's staff, she will say that Dragowrath is near but he's only found by "true magic from a true magician" or something hinting at Merlin</t>
+  </si>
+  <si>
+    <t>Once the player reached all the prerequisites, she'll say that a magical portal opened up which is in the same cave system end, and going through tps to Dragowrath on remote island</t>
+  </si>
+  <si>
+    <t>Now once the player goes back to Nova with Dragowrath on their team, she'll help Dragowrath summon one of the 6 Ultra Paradox mons to catch at a random spot on the island</t>
+  </si>
+  <si>
+    <t>The POI guardians (Diftery for Shadow Path/Shadow Ravine/Electric Tunnel), Triwandoliz (Mt Splinkty), Soarwhell (Mindagan Lake) are catchable but need their items to summon them</t>
+  </si>
+  <si>
+    <t>Kleinyeti is obtainable by getting the spaceship to crash on a commercial ride back from Space and crash landing at Mystery Peak, where one will spawn there</t>
+  </si>
+  <si>
+    <t>Solaroxyous is only obtainable by completing the dex (except it), then I (Shae) spawns in (TBD), and upon beating me I give you the fallen star, which will summon at peak of Mt St Joseph</t>
   </si>
 </sst>
 </file>
@@ -1553,16 +1589,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:AD142"/>
+  <dimension ref="A1:AD154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="AD33" sqref="AD33"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="AB35" sqref="AB35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="153.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="165" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3317,6 +3353,66 @@
         <v>196</v>
       </c>
     </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commercial outer space, casino revamp, Mystery Peak done!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/xhenos story work.xlsx
+++ b/PokemonGame/stuff/xhenos story work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C6B1F2-D620-421A-A6DA-F0C1F27292B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE23ECD-090F-4281-BADA-D66D22CBCBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="397">
   <si>
     <t>Current</t>
   </si>
@@ -1215,6 +1215,18 @@
   </si>
   <si>
     <t>Coins Update</t>
+  </si>
+  <si>
+    <t>Mystery Peak</t>
+  </si>
+  <si>
+    <t>Space Back</t>
+  </si>
+  <si>
+    <t>All V Forms</t>
+  </si>
+  <si>
+    <t>Perilyte 1</t>
   </si>
 </sst>
 </file>
@@ -1594,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AD154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,6 +2153,9 @@
       <c r="T27" t="s">
         <v>289</v>
       </c>
+      <c r="U27" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2449,7 +2464,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2498,8 +2513,17 @@
       <c r="P33" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>394</v>
+      </c>
+      <c r="R33" t="s">
+        <v>393</v>
+      </c>
+      <c r="S33" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2516,7 +2540,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2530,7 +2554,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2544,7 +2568,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +2582,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2572,7 +2596,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2586,7 +2610,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2600,7 +2624,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2614,7 +2638,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2628,7 +2652,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2642,7 +2666,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2656,7 +2680,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2670,7 +2694,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2684,7 +2708,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2698,7 +2722,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>

</xml_diff>